<commit_message>
Write up of test cases
</commit_message>
<xml_diff>
--- a/HW 3/Test Cases.xlsx
+++ b/HW 3/Test Cases.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS2080C\GitHub\DataStructures-Group12\HW 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\source\repos\DataStructures-Group12\HW 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F554350E-FCCA-482D-9232-547BDDDCD807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFAC197-7780-4F8B-A0A1-6F7B38FF524C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
   <si>
     <t>Test Case #</t>
   </si>
@@ -55,6 +56,606 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Designed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Caleb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Designed Date: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>03/09/2020</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Executed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keith</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Execution Date: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>03/10/2020</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Designed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Brandon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Executed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Manvith</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Designed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Keith</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Executed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Brandon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Designed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Manvith</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Executed By: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Caleb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Priority: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medium</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Module Name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>War.cpp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Case ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TC_P_SE_1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peek top card when side deck is empty</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test the peeking option when the side deck is empty</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Player side pile is empty and they choose to peek</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dependencies: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>None</t>
+    </r>
+  </si>
+  <si>
+    <t>Choose to peek</t>
+  </si>
+  <si>
+    <t>Choose to place the card on side pile</t>
+  </si>
+  <si>
+    <t>Showed pulled card</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Put card in side</t>
+  </si>
+  <si>
+    <t>Play the next card in the deck</t>
+  </si>
+  <si>
+    <t>Played the next card</t>
+  </si>
+  <si>
+    <t>User was not allowed to pull from side when it was empty, which is expected</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Case ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TC_P_SF_2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peek top card when side deck is full</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test the peeking option when the side deck is full</t>
+    </r>
+  </si>
+  <si>
+    <t>Pull from side pile</t>
+  </si>
+  <si>
+    <t>Pulled from side pile</t>
+  </si>
+  <si>
+    <t>Play the side card</t>
+  </si>
+  <si>
+    <t>Played the side card</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Player side pile is full and they choose to peek</t>
+    </r>
+  </si>
+  <si>
+    <t>User was not allowed to put onto the side pile since it was full, which is expected</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Post-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Player is able to play the next card on deck and the result of the round is displayed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Post-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Player is able to play the side card with pulled card and result of round is displayed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Priority: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>High</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Case ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TC_NP_3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No peek and playing next card in deck</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test not peeking and simply playing the next card in deck</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Playing the game, not choosing to peek</t>
+    </r>
+  </si>
+  <si>
+    <t>Choose not to peek</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Player plays next card</t>
+  </si>
+  <si>
+    <t>Player played next card</t>
+  </si>
+  <si>
+    <t>Player was not shown the next card and the next card was simply played</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Post-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Card was played without being shown to the player first and round result is displayed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Case ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TC_R_GO_4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Title: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last round finished in rounds mode</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test when the last round is completed when playing in the round mode of the game</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Player chose rounds mode of game and is in the last round</t>
+    </r>
+  </si>
+  <si>
+    <t>End of Game</t>
+  </si>
+  <si>
+    <t>Game Ends</t>
+  </si>
+  <si>
+    <t>Game Ended</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Game ended after last round and result of the game was displayed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Post-Conditions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Game ends and game result is displayed</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -86,7 +687,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -109,17 +710,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,4 +1267,874 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61423A1-BCFA-4799-B1AE-ECBEECBB9105}">
+  <dimension ref="C7:Q41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" customWidth="1"/>
+    <col min="16" max="16" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="K8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="18"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="K9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="K10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="K11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="15"/>
+    </row>
+    <row r="12" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="K12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="12"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="K14" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="K15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="12"/>
+    </row>
+    <row r="16" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="21"/>
+    </row>
+    <row r="17" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="6">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="7">
+        <v>7</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="29"/>
+      <c r="K19" s="6">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" s="29"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C20" s="6">
+        <v>3</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="7">
+        <v>10</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="29"/>
+      <c r="K20" s="6">
+        <v>3</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="7">
+        <v>5</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P20" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="29"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="29"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="29"/>
+    </row>
+    <row r="22" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="30"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="30"/>
+    </row>
+    <row r="23" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="K23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="12"/>
+    </row>
+    <row r="25" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C26" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+      <c r="K26" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="18"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C27" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
+      <c r="K27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="15"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="15"/>
+      <c r="K28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C29" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
+      <c r="K29" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="15"/>
+    </row>
+    <row r="30" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
+      <c r="K30" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="12"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="5"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C32" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="15"/>
+      <c r="K32" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="15"/>
+    </row>
+    <row r="33" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+      <c r="K33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="12"/>
+    </row>
+    <row r="34" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="21"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="21"/>
+    </row>
+    <row r="35" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O35" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="P35" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q35" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="6">
+        <v>1</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P36" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="32"/>
+      <c r="K37" s="6">
+        <v>2</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P37" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q37" s="29"/>
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="32"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="29"/>
+    </row>
+    <row r="39" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="32"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="29"/>
+    </row>
+    <row r="40" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="33"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="30"/>
+    </row>
+    <row r="41" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="12"/>
+      <c r="K41" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="61">
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="K12:Q12"/>
+    <mergeCell ref="Q18:Q22"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="Q36:Q40"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="K33:Q33"/>
+    <mergeCell ref="K34:Q34"/>
+    <mergeCell ref="K41:Q41"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="K31:Q31"/>
+    <mergeCell ref="K32:Q32"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="O28:Q28"/>
+    <mergeCell ref="K13:Q13"/>
+    <mergeCell ref="K14:Q14"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="K16:Q16"/>
+    <mergeCell ref="K23:Q23"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>